<commit_message>
updated tourism goal, running smoothly now. Added information on forest health/watershed health
</commit_message>
<xml_diff>
--- a/prep/goal tables.xlsx
+++ b/prep/goal tables.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="900" windowWidth="23235" windowHeight="9180" activeTab="3"/>
+    <workbookView xWindow="840" yWindow="900" windowWidth="23235" windowHeight="9180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="AO" sheetId="1" r:id="rId1"/>
     <sheet name="LIV" sheetId="2" r:id="rId2"/>
     <sheet name="ECO" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="SPP" sheetId="4" r:id="rId4"/>
+    <sheet name="T" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
   <si>
     <t>region_id</t>
   </si>
@@ -85,7 +86,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +111,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -123,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -133,6 +140,8 @@
     <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,10 +707,10 @@
         <v>7</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -758,6 +767,81 @@
       </c>
       <c r="D5" s="4">
         <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>61.9</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-0.29110000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-0.24629999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>56</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-0.39589999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1">
+        <v>59.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-0.39689999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated layout of flower plots
</commit_message>
<xml_diff>
--- a/prep/goal tables.xlsx
+++ b/prep/goal tables.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="900" windowWidth="23235" windowHeight="9180" activeTab="4"/>
+    <workbookView xWindow="840" yWindow="900" windowWidth="23235" windowHeight="9180" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="AO" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="ECO" sheetId="3" r:id="rId3"/>
     <sheet name="SPP" sheetId="4" r:id="rId4"/>
     <sheet name="T" sheetId="5" r:id="rId5"/>
+    <sheet name="BD" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="38">
   <si>
     <t>region_id</t>
   </si>
@@ -60,13 +61,88 @@
   </si>
   <si>
     <t>goal</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>rgn_id</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>score e</t>
+  </si>
+  <si>
+    <t>nv_score</t>
+  </si>
+  <si>
+    <t>n_score</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>Economic</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>beach</t>
+  </si>
+  <si>
+    <t>reef</t>
+  </si>
+  <si>
+    <t>soft-bottom</t>
+  </si>
+  <si>
+    <t>watershed</t>
+  </si>
+  <si>
+    <t>wetland</t>
+  </si>
+  <si>
+    <t>Habitat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference </t>
+  </si>
+  <si>
+    <t>% acreation</t>
+  </si>
+  <si>
+    <t>%CC, %CA, %MA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% area unimpacted by dredging </t>
+  </si>
+  <si>
+    <t>30% of priority watersheds protected</t>
+  </si>
+  <si>
+    <t>no historic extent data = 50%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +161,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,8 +205,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,11 +226,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -142,6 +251,24 @@
     <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,19 +904,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="17" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -799,8 +932,17 @@
       <c r="C1" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -810,8 +952,17 @@
       <c r="C2" s="1">
         <v>-0.29110000000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G2" s="14">
+        <v>63.542400000000001</v>
+      </c>
+      <c r="H2" s="14">
+        <v>45.580735000000004</v>
+      </c>
+      <c r="I2" s="14">
+        <v>79.665359499999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -822,7 +973,7 @@
         <v>-0.24629999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -833,7 +984,7 @@
         <v>-0.39589999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -844,8 +995,902 @@
         <v>-0.39689999999999998</v>
       </c>
     </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="11">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D12" s="1">
+        <v>67.461749999999995</v>
+      </c>
+      <c r="E12" s="1">
+        <v>41.946820000000002</v>
+      </c>
+      <c r="F12" s="1">
+        <v>100</v>
+      </c>
+      <c r="G12" s="1">
+        <v>69.802859999999995</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="14">
+        <f>AVERAGE(D12:D16)</f>
+        <v>63.542400000000001</v>
+      </c>
+      <c r="J12" s="14">
+        <f>AVERAGE(E12:E16)</f>
+        <v>41.946820000000002</v>
+      </c>
+      <c r="K12" s="14">
+        <f>AVERAGE(F12:F16)</f>
+        <v>80.259478000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D13" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E13" s="1">
+        <v>41.946820000000002</v>
+      </c>
+      <c r="F13" s="1">
+        <v>100</v>
+      </c>
+      <c r="G13" s="1">
+        <v>67.73227</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="14">
+        <f>AVERAGE(D17:D21)</f>
+        <v>63.542400000000001</v>
+      </c>
+      <c r="J13" s="14">
+        <f t="shared" ref="J13:K13" si="0">AVERAGE(E17:E21)</f>
+        <v>71.866669999999999</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="0"/>
+        <v>88.401960000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="11">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D14" s="1">
+        <v>64.000249999999994</v>
+      </c>
+      <c r="E14" s="1">
+        <v>41.946820000000002</v>
+      </c>
+      <c r="F14" s="1">
+        <v>63.311979999999998</v>
+      </c>
+      <c r="G14" s="1">
+        <v>56.41968</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="14">
+        <f>AVERAGE(D22:D26)</f>
+        <v>63.542400000000001</v>
+      </c>
+      <c r="J14" s="14">
+        <f t="shared" ref="J14:K14" si="1">AVERAGE(E22:E26)</f>
+        <v>34.510840000000002</v>
+      </c>
+      <c r="K14" s="14">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D15" s="1">
+        <v>63.75</v>
+      </c>
+      <c r="E15" s="1">
+        <v>41.946820000000002</v>
+      </c>
+      <c r="F15" s="1">
+        <v>87.985410000000002</v>
+      </c>
+      <c r="G15" s="1">
+        <v>64.560739999999996</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15" s="17">
+        <f>AVERAGE(D27:D31)</f>
+        <v>63.542400000000001</v>
+      </c>
+      <c r="J15" s="17">
+        <f t="shared" ref="J15:L15" si="2">AVERAGE(E27:E31)</f>
+        <v>33.998609999999999</v>
+      </c>
+      <c r="K15" s="17">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="11">
+        <v>5</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D16" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E16" s="1">
+        <v>41.946820000000002</v>
+      </c>
+      <c r="F16" s="1">
+        <v>50</v>
+      </c>
+      <c r="G16" s="1">
+        <v>51.06561</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I16" s="14">
+        <f>AVERAGE(I12:I15)</f>
+        <v>63.542400000000001</v>
+      </c>
+      <c r="J16" s="14">
+        <f t="shared" ref="J16:K16" si="3">AVERAGE(J12:J15)</f>
+        <v>45.580735000000004</v>
+      </c>
+      <c r="K16" s="14">
+        <f t="shared" si="3"/>
+        <v>79.665359499999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="11">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D17" s="1">
+        <v>67.461749999999995</v>
+      </c>
+      <c r="E17" s="1">
+        <v>71.866669999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>100</v>
+      </c>
+      <c r="G17" s="1">
+        <v>79.776139999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="11">
+        <v>7</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D18" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E18" s="1">
+        <v>71.866669999999999</v>
+      </c>
+      <c r="F18" s="1">
+        <v>100</v>
+      </c>
+      <c r="G18" s="1">
+        <v>77.705560000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="11">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D19" s="1">
+        <v>64.000249999999994</v>
+      </c>
+      <c r="E19" s="1">
+        <v>71.866669999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>100</v>
+      </c>
+      <c r="G19" s="1">
+        <v>78.622309999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D20" s="1">
+        <v>63.75</v>
+      </c>
+      <c r="E20" s="1">
+        <v>71.866669999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>92.009799999999998</v>
+      </c>
+      <c r="G20" s="1">
+        <v>75.875489999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="11">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D21" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E21" s="1">
+        <v>71.866669999999999</v>
+      </c>
+      <c r="F21" s="1">
+        <v>50</v>
+      </c>
+      <c r="G21" s="1">
+        <v>61.038890000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="11">
+        <v>11</v>
+      </c>
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D22" s="1">
+        <v>67.461749999999995</v>
+      </c>
+      <c r="E22" s="1">
+        <v>34.510840000000002</v>
+      </c>
+      <c r="F22" s="1">
+        <v>100</v>
+      </c>
+      <c r="G22" s="1">
+        <v>67.324200000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="11">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D23" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E23" s="1">
+        <v>34.510840000000002</v>
+      </c>
+      <c r="F23" s="1">
+        <v>100</v>
+      </c>
+      <c r="G23" s="1">
+        <v>65.253609999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="11">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D24" s="1">
+        <v>64.000249999999994</v>
+      </c>
+      <c r="E24" s="1">
+        <v>34.510840000000002</v>
+      </c>
+      <c r="F24" s="1">
+        <v>50</v>
+      </c>
+      <c r="G24" s="1">
+        <v>49.503700000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="11">
+        <v>14</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D25" s="1">
+        <v>63.75</v>
+      </c>
+      <c r="E25" s="1">
+        <v>34.510840000000002</v>
+      </c>
+      <c r="F25" s="1">
+        <v>50</v>
+      </c>
+      <c r="G25" s="1">
+        <v>49.420279999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="11">
+        <v>15</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D26" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E26" s="1">
+        <v>34.510840000000002</v>
+      </c>
+      <c r="F26" s="1">
+        <v>50</v>
+      </c>
+      <c r="G26" s="1">
+        <v>48.586950000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="11">
+        <v>16</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2011</v>
+      </c>
+      <c r="D27" s="1">
+        <v>67.461749999999995</v>
+      </c>
+      <c r="E27" s="1">
+        <v>33.998609999999999</v>
+      </c>
+      <c r="F27" s="1">
+        <v>100</v>
+      </c>
+      <c r="G27" s="1">
+        <v>67.153450000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="11">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2012</v>
+      </c>
+      <c r="D28" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E28" s="1">
+        <v>33.998609999999999</v>
+      </c>
+      <c r="F28" s="1">
+        <v>100</v>
+      </c>
+      <c r="G28" s="1">
+        <v>65.08287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2013</v>
+      </c>
+      <c r="D29" s="1">
+        <v>64.000249999999994</v>
+      </c>
+      <c r="E29" s="1">
+        <v>33.998609999999999</v>
+      </c>
+      <c r="F29" s="1">
+        <v>100</v>
+      </c>
+      <c r="G29" s="1">
+        <v>65.999619999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="11">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D30" s="1">
+        <v>63.75</v>
+      </c>
+      <c r="E30" s="1">
+        <v>33.998609999999999</v>
+      </c>
+      <c r="F30" s="1">
+        <v>50</v>
+      </c>
+      <c r="G30" s="1">
+        <v>49.249540000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="11">
+        <v>20</v>
+      </c>
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2015</v>
+      </c>
+      <c r="D31" s="1">
+        <v>61.25</v>
+      </c>
+      <c r="E31" s="1">
+        <v>33.998609999999999</v>
+      </c>
+      <c r="F31" s="1">
+        <v>50</v>
+      </c>
+      <c r="G31" s="1">
+        <v>48.416200000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="12"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="20"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="20">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="20">
+        <v>81</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="20">
+        <v>61</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="20">
+        <v>40.160310000000003</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="20">
+        <v>50</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="20">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="20">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="20">
+        <v>98</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="20">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="20">
+        <v>50</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="20">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="20">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="20">
+        <v>49</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="20">
+        <v>25.288350000000001</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="20">
+        <v>50</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="20">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="20">
+        <v>61</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="20">
+        <v>99</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="20">
+        <v>24.26388</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="20">
+        <v>50</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>